<commit_message>
General formatting and adding imports
</commit_message>
<xml_diff>
--- a/Weather_Tracker.xlsx
+++ b/Weather_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1335" yWindow="3540" windowWidth="23430" windowHeight="9300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Weather" sheetId="1" state="visible" r:id="rId1"/>
@@ -461,10 +461,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q118"/>
+  <dimension ref="A1:Q120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N82" sqref="N82"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U94" sqref="U94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -523,7 +523,7 @@
         </is>
       </c>
       <c r="Q1" t="n">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2">
@@ -3411,10 +3411,8 @@
           <t>102.2kPa</t>
         </is>
       </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>31%</t>
-        </is>
+      <c r="G85" s="1" t="n">
+        <v>0.31</v>
       </c>
       <c r="I85" t="inlineStr">
         <is>
@@ -3449,10 +3447,8 @@
           <t>101.7kPa</t>
         </is>
       </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>29%</t>
-        </is>
+      <c r="G86" s="1" t="n">
+        <v>0.29</v>
       </c>
       <c r="I86" t="inlineStr">
         <is>
@@ -3487,10 +3483,8 @@
           <t>101.8kPa</t>
         </is>
       </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>43%</t>
-        </is>
+      <c r="G87" s="1" t="n">
+        <v>0.43</v>
       </c>
       <c r="I87" t="inlineStr">
         <is>
@@ -3525,10 +3519,8 @@
           <t>101.7kPa</t>
         </is>
       </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>31%</t>
-        </is>
+      <c r="G88" s="1" t="n">
+        <v>0.31</v>
       </c>
       <c r="I88" t="inlineStr">
         <is>
@@ -3563,10 +3555,8 @@
           <t>101.7kPa</t>
         </is>
       </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>45%</t>
-        </is>
+      <c r="G89" s="1" t="n">
+        <v>0.45</v>
       </c>
       <c r="I89" t="inlineStr">
         <is>
@@ -3601,10 +3591,8 @@
           <t>102.0kPa</t>
         </is>
       </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>62%</t>
-        </is>
+      <c r="G90" s="1" t="n">
+        <v>0.62</v>
       </c>
       <c r="I90" t="inlineStr">
         <is>
@@ -3639,10 +3627,8 @@
           <t>101.9kPa</t>
         </is>
       </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>57%</t>
-        </is>
+      <c r="G91" s="1" t="n">
+        <v>0.57</v>
       </c>
       <c r="I91" t="inlineStr">
         <is>
@@ -3677,10 +3663,8 @@
           <t>101.9kPa</t>
         </is>
       </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>68%</t>
-        </is>
+      <c r="G92" s="1" t="n">
+        <v>0.68</v>
       </c>
       <c r="I92" t="inlineStr">
         <is>
@@ -3715,10 +3699,8 @@
           <t>102.1kPa</t>
         </is>
       </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>85%</t>
-        </is>
+      <c r="G93" s="1" t="n">
+        <v>0.85</v>
       </c>
       <c r="I93" t="inlineStr">
         <is>
@@ -3753,10 +3735,8 @@
           <t>101.9kPa</t>
         </is>
       </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>67%</t>
-        </is>
+      <c r="G94" s="1" t="n">
+        <v>0.67</v>
       </c>
       <c r="I94" t="inlineStr">
         <is>
@@ -3791,10 +3771,8 @@
           <t>101.5kPa</t>
         </is>
       </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>32%</t>
-        </is>
+      <c r="G95" s="1" t="n">
+        <v>0.32</v>
       </c>
       <c r="I95" t="inlineStr">
         <is>
@@ -3829,10 +3807,8 @@
           <t>100.8kPa</t>
         </is>
       </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>48%</t>
-        </is>
+      <c r="G96" s="1" t="n">
+        <v>0.48</v>
       </c>
       <c r="I96" t="inlineStr">
         <is>
@@ -3867,10 +3843,8 @@
           <t>101.2kPa</t>
         </is>
       </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>46%</t>
-        </is>
+      <c r="G97" s="1" t="n">
+        <v>0.46</v>
       </c>
       <c r="I97" t="inlineStr">
         <is>
@@ -3905,10 +3879,8 @@
           <t>101.2kPa</t>
         </is>
       </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>86%</t>
-        </is>
+      <c r="G98" s="1" t="n">
+        <v>0.86</v>
       </c>
       <c r="I98" t="inlineStr">
         <is>
@@ -3941,10 +3913,8 @@
           <t>100.9kPa</t>
         </is>
       </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>93%</t>
-        </is>
+      <c r="G99" s="1" t="n">
+        <v>0.93</v>
       </c>
       <c r="I99" t="inlineStr">
         <is>
@@ -3979,10 +3949,8 @@
           <t>100.4kPa</t>
         </is>
       </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>47%</t>
-        </is>
+      <c r="G100" s="1" t="n">
+        <v>0.47</v>
       </c>
       <c r="I100" t="inlineStr">
         <is>
@@ -4017,10 +3985,8 @@
           <t>101.1kPa</t>
         </is>
       </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>47%</t>
-        </is>
+      <c r="G101" s="1" t="n">
+        <v>0.47</v>
       </c>
       <c r="I101" t="inlineStr">
         <is>
@@ -4055,10 +4021,8 @@
           <t>100.8kPa</t>
         </is>
       </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>63%</t>
-        </is>
+      <c r="G102" s="1" t="n">
+        <v>0.63</v>
       </c>
       <c r="I102" t="inlineStr">
         <is>
@@ -4093,10 +4057,8 @@
           <t>100.6kPa</t>
         </is>
       </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>80%</t>
-        </is>
+      <c r="G103" s="1" t="n">
+        <v>0.8</v>
       </c>
       <c r="I103" t="inlineStr">
         <is>
@@ -4131,10 +4093,8 @@
           <t>101.3kPa</t>
         </is>
       </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>27%</t>
-        </is>
+      <c r="G104" s="1" t="n">
+        <v>0.27</v>
       </c>
       <c r="I104" t="inlineStr">
         <is>
@@ -4169,10 +4129,8 @@
           <t>101.4kPa</t>
         </is>
       </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>74%</t>
-        </is>
+      <c r="G105" s="1" t="n">
+        <v>0.74</v>
       </c>
       <c r="I105" t="inlineStr">
         <is>
@@ -4207,10 +4165,8 @@
           <t>101.3kPa</t>
         </is>
       </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>68%</t>
-        </is>
+      <c r="G106" s="1" t="n">
+        <v>0.68</v>
       </c>
       <c r="I106" t="inlineStr">
         <is>
@@ -4245,10 +4201,8 @@
           <t>101.4kPa</t>
         </is>
       </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>56%</t>
-        </is>
+      <c r="G107" s="1" t="n">
+        <v>0.5600000000000001</v>
       </c>
       <c r="I107" t="inlineStr">
         <is>
@@ -4283,10 +4237,8 @@
           <t>101.3kPa</t>
         </is>
       </c>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>73%</t>
-        </is>
+      <c r="G108" s="1" t="n">
+        <v>0.73</v>
       </c>
       <c r="I108" t="inlineStr">
         <is>
@@ -4321,10 +4273,8 @@
           <t>101.8kPa</t>
         </is>
       </c>
-      <c r="G109" t="inlineStr">
-        <is>
-          <t>32%</t>
-        </is>
+      <c r="G109" s="1" t="n">
+        <v>0.32</v>
       </c>
       <c r="I109" t="inlineStr">
         <is>
@@ -4359,10 +4309,8 @@
           <t>101.0kPa</t>
         </is>
       </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>25%</t>
-        </is>
+      <c r="G110" s="1" t="n">
+        <v>0.25</v>
       </c>
       <c r="I110" t="inlineStr">
         <is>
@@ -4397,10 +4345,8 @@
           <t>100.7kPa</t>
         </is>
       </c>
-      <c r="G111" t="inlineStr">
-        <is>
-          <t>69%</t>
-        </is>
+      <c r="G111" s="1" t="n">
+        <v>0.6899999999999999</v>
       </c>
       <c r="I111" t="inlineStr">
         <is>
@@ -4435,10 +4381,8 @@
           <t>100.7kPa</t>
         </is>
       </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>49%</t>
-        </is>
+      <c r="G112" s="1" t="n">
+        <v>0.49</v>
       </c>
       <c r="I112" t="inlineStr">
         <is>
@@ -4473,10 +4417,8 @@
           <t>99.6kPa</t>
         </is>
       </c>
-      <c r="G113" t="inlineStr">
-        <is>
-          <t>83%</t>
-        </is>
+      <c r="G113" s="1" t="n">
+        <v>0.83</v>
       </c>
       <c r="I113" t="inlineStr">
         <is>
@@ -4511,10 +4453,8 @@
           <t>101.7kPa</t>
         </is>
       </c>
-      <c r="G114" t="inlineStr">
-        <is>
-          <t>74%</t>
-        </is>
+      <c r="G114" s="1" t="n">
+        <v>0.74</v>
       </c>
       <c r="I114" t="inlineStr">
         <is>
@@ -4549,10 +4489,8 @@
           <t>101.7kPa</t>
         </is>
       </c>
-      <c r="G115" t="inlineStr">
-        <is>
-          <t>85%</t>
-        </is>
+      <c r="G115" s="1" t="n">
+        <v>0.85</v>
       </c>
       <c r="I115" t="inlineStr">
         <is>
@@ -4587,10 +4525,8 @@
           <t>101.3kPa</t>
         </is>
       </c>
-      <c r="G116" t="inlineStr">
-        <is>
-          <t>46%</t>
-        </is>
+      <c r="G116" s="1" t="n">
+        <v>0.46</v>
       </c>
       <c r="I116" t="inlineStr">
         <is>
@@ -4625,10 +4561,8 @@
           <t>101.4kPa</t>
         </is>
       </c>
-      <c r="G117" t="inlineStr">
-        <is>
-          <t>59%</t>
-        </is>
+      <c r="G117" s="1" t="n">
+        <v>0.59</v>
       </c>
       <c r="I117" t="inlineStr">
         <is>
@@ -4663,10 +4597,8 @@
           <t>102.0kPa</t>
         </is>
       </c>
-      <c r="G118" t="inlineStr">
-        <is>
-          <t>73%</t>
-        </is>
+      <c r="G118" s="1" t="n">
+        <v>0.73</v>
       </c>
       <c r="I118" t="inlineStr">
         <is>
@@ -4685,6 +4617,76 @@
       </c>
       <c r="O118" t="n">
         <v>24</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>-1.4</v>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>MostlyCloudy</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>101.3kPa</t>
+        </is>
+      </c>
+      <c r="G119" s="1" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>WNW17km/h</t>
+        </is>
+      </c>
+      <c r="K119" t="n">
+        <v>-7</v>
+      </c>
+      <c r="M119" t="inlineStr">
+        <is>
+          <t>2021-12-26 12:01</t>
+        </is>
+      </c>
+      <c r="O119" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>-1.4</v>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>MostlyCloudy</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>101.3kPa</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>72%</t>
+        </is>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>WNW17km/h</t>
+        </is>
+      </c>
+      <c r="K120" t="n">
+        <v>-7</v>
+      </c>
+      <c r="M120" t="inlineStr">
+        <is>
+          <t>2021-12-26 12:04</t>
+        </is>
+      </c>
+      <c r="O120" t="n">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>